<commit_message>
Latest canvas course groups small cleanup in .r file
fixed typos in the blank templates
</commit_message>
<xml_diff>
--- a/PeerEvaluationTemplate_2Person.xlsx
+++ b/PeerEvaluationTemplate_2Person.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\walterm\Dropbox\Classes\MAE151W22\GradesRosters\PeerEval\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\walterm\Documents\GitProjects\PeerEvalTemplateCreator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8AAAF325-E0E7-4298-B9B2-44192C59DD6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFBEA1FB-3362-4DC7-B050-B690971C0C73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="825" yWindow="-120" windowWidth="23295" windowHeight="13740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="PeerRating" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -26,17 +25,7 @@
     <t>Category</t>
   </si>
   <si>
-    <t>Rating Descriptions (provide whole number ratings (5, 4, 3, 2, or 1) in columns for each each member including yourself)</t>
-  </si>
-  <si>
     <t>Having Relevant Knowledge, Skills, and Abilities (KSAs)</t>
-  </si>
-  <si>
-    <t>5: Demonstrates KSAs to do excellent work, acquires new KSA to help team, can perform any role on team if necessary
-4: Between 5 above and 3 below
-3: Demonstrates sufficient KSA to contribute to team, acquires KSAs to meet requirements, able to perform other tasks
-2: Between 3 above and 1 below
-1: Missing basic qualification, unable to develop KSAs to contribute to team, unable to peform any one elses duties</t>
   </si>
   <si>
     <t>Contributing to the Team’s Work</t>
@@ -50,25 +39,10 @@
     <t>Interacting with Teammates</t>
   </si>
   <si>
-    <t>5: Is interested in teammates ideas and contributions, makes sure everyone is informed, is encouraging, enthusiastic and asks for feedback/suggestions
-3: Listens and respects teammate contributsions, communicates clearly, shares info, participates fully, reacts and responds to feedback/suggestions
-1: Interrupts, ignores, bosses, or makes fun, takes action without input, does not share, complains, makes excuses, does not interact, is defensive</t>
-  </si>
-  <si>
     <t>Keeping the Team on Track</t>
   </si>
   <si>
-    <t>5: Monitors teams' progress, makes sure teammates are progressing, gives specific, timely, and constructive feedback
-3: Knows what everyone on the team should be doing and notices problems, alerts teammates and suggests solutions with sucess is threatened
-1: Unaware if team is meeting goals, does not pay attention to teammates progress, avoids discussing team problems even when obvious</t>
-  </si>
-  <si>
     <t>Expecting Quality</t>
-  </si>
-  <si>
-    <t>5: Motivates team to do excellent work, cares about excellent work even without reward, believes in team's ability to do excellent work
-3: Encouarges good work to meet requirements, believes team can meet its responsiblities
-1: Satisfied even if not all requirements are met,  avoids work, doubts team can meet requirements</t>
   </si>
   <si>
     <t xml:space="preserve">Comments (REQUIRED): For each person (including yourself), in the corresponding shaded box below, comment on how the teammate can improve on his/her worst rating </t>
@@ -78,6 +52,31 @@
   </si>
   <si>
     <t xml:space="preserve">&lt;-- B2 Person </t>
+  </si>
+  <si>
+    <t>5: Demonstrates KSAs to do excellent work, acquires new KSA to help team, can perform any role on team if necessary
+4: Between 5 above and 3 below
+3: Demonstrates sufficient KSA to contribute to team, acquires KSAs to meet requirements, able to perform other tasks
+2: Between 3 above and 1 below
+1: Missing basic qualification, unable to develop KSAs to contribute to team, unable to perform any one else's duties</t>
+  </si>
+  <si>
+    <t>5: Is interested in teammates ideas and contributions, makes sure everyone is informed, is encouraging, enthusiastic and asks for feedback/suggestions
+3: Listens and respects teammate contributions, communicates clearly, shares info, participates fully, reacts and responds to feedback/suggestions
+1: Interrupts, ignores, bosses, or makes fun, takes action without input, does not share, complains, makes excuses, does not interact, is defensive</t>
+  </si>
+  <si>
+    <t>5: Monitors teams' progress, makes sure teammates are progressing, gives specific, timely, and constructive feedback
+3: Knows what everyone on the team should be doing and notices problems, alerts teammates and suggests solutions with success is threatened
+1: Unaware if team is meeting goals, does not pay attention to teammates progress, avoids discussing team problems even when obvious</t>
+  </si>
+  <si>
+    <t>5: Motivates team to do excellent work, cares about excellent work even without reward, believes in team's ability to do excellent work
+3: Encourages good work to meet requirements, believes team can meet its responsibilities
+1: Satisfied even if not all requirements are met,  avoids work, doubts team can meet requirements</t>
+  </si>
+  <si>
+    <t>Rating Descriptions (provide whole number ratings (5, 4, 3, 2, or 1) in columns for each member including yourself)</t>
   </si>
 </sst>
 </file>
@@ -305,13 +304,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -342,8 +341,7 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -354,10 +352,10 @@
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -378,9 +376,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -418,7 +416,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -524,7 +522,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -666,7 +664,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -680,7 +678,7 @@
   <dimension ref="A1:U992"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -691,10 +689,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="19"/>
-      <c r="B1" s="20"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="22"/>
+      <c r="A1" s="18"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="21"/>
     </row>
     <row r="2" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2"/>
@@ -709,17 +707,17 @@
         <v>0</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>1</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:21" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="9" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E4" s="11"/>
       <c r="F4" s="11"/>
@@ -743,10 +741,10 @@
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="12" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E5" s="11"/>
       <c r="F5" s="11"/>
@@ -770,10 +768,10 @@
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="14" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E6" s="11"/>
       <c r="F6" s="11"/>
@@ -797,10 +795,10 @@
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="9" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E7" s="11"/>
       <c r="F7" s="11"/>
@@ -824,10 +822,10 @@
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="9" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E8" s="11"/>
       <c r="F8" s="11"/>
@@ -849,78 +847,26 @@
     </row>
     <row r="9" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="16" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
-      <c r="B9" s="17"/>
-      <c r="C9" s="17"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="17"/>
-      <c r="G9" s="17"/>
-      <c r="H9" s="17"/>
-      <c r="I9" s="17"/>
-      <c r="J9" s="17"/>
-      <c r="K9" s="17"/>
-      <c r="L9" s="17"/>
-      <c r="M9" s="17"/>
-      <c r="N9" s="17"/>
-      <c r="O9" s="17"/>
-      <c r="P9" s="17"/>
-      <c r="Q9" s="17"/>
-      <c r="R9" s="17"/>
-      <c r="S9" s="17"/>
-      <c r="T9" s="17"/>
-      <c r="U9" s="17"/>
+      <c r="D9" s="17"/>
     </row>
     <row r="10" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="23"/>
-      <c r="B10" s="24"/>
-      <c r="C10" s="24"/>
-      <c r="D10" s="25"/>
-      <c r="E10" s="17" t="s">
-        <v>13</v>
+      <c r="A10" s="22"/>
+      <c r="B10" s="23"/>
+      <c r="C10" s="23"/>
+      <c r="D10" s="24"/>
+      <c r="E10" t="s">
+        <v>8</v>
       </c>
-      <c r="F10" s="17"/>
-      <c r="G10" s="17"/>
-      <c r="H10" s="17"/>
-      <c r="I10" s="17"/>
-      <c r="J10" s="17"/>
-      <c r="K10" s="17"/>
-      <c r="L10" s="17"/>
-      <c r="M10" s="17"/>
-      <c r="N10" s="17"/>
-      <c r="O10" s="17"/>
-      <c r="P10" s="17"/>
-      <c r="Q10" s="17"/>
-      <c r="R10" s="17"/>
-      <c r="S10" s="17"/>
-      <c r="T10" s="17"/>
-      <c r="U10" s="17"/>
     </row>
     <row r="11" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="17"/>
-      <c r="B11" s="23"/>
-      <c r="C11" s="24"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="17" t="s">
-        <v>14</v>
+      <c r="B11" s="22"/>
+      <c r="C11" s="23"/>
+      <c r="D11" s="24"/>
+      <c r="E11" t="s">
+        <v>9</v>
       </c>
-      <c r="F11" s="17"/>
-      <c r="G11" s="17"/>
-      <c r="H11" s="17"/>
-      <c r="I11" s="17"/>
-      <c r="J11" s="17"/>
-      <c r="K11" s="17"/>
-      <c r="L11" s="17"/>
-      <c r="M11" s="17"/>
-      <c r="N11" s="17"/>
-      <c r="O11" s="17"/>
-      <c r="P11" s="17"/>
-      <c r="Q11" s="17"/>
-      <c r="R11" s="17"/>
-      <c r="S11" s="17"/>
-      <c r="T11" s="17"/>
-      <c r="U11" s="17"/>
     </row>
     <row r="12" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="13" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>